<commit_message>
interfaz - web - tablet
</commit_message>
<xml_diff>
--- a/emprenidmineto/flujo_efetivo.xlsx
+++ b/emprenidmineto/flujo_efetivo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erikG\Documents\ciclo2025-1\materias-ciclo-2025-1\emprenidmineto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD0AFAD-65D0-45D3-ABB3-BD44CA45D08E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6B69A6-0DEE-4C5E-A764-2718AC79CB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{97FEF6D0-0AE0-4C10-9DE4-DC0CBDD2AAA0}"/>
   </bookViews>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>salidas</t>
   </si>
   <si>
-    <t>costo</t>
-  </si>
-  <si>
     <t>renta</t>
   </si>
   <si>
@@ -57,6 +54,39 @@
   </si>
   <si>
     <t>registro de marca/logo</t>
+  </si>
+  <si>
+    <t>costo (USD)</t>
+  </si>
+  <si>
+    <t>6500 - 13000</t>
+  </si>
+  <si>
+    <t>100-300</t>
+  </si>
+  <si>
+    <t>internet</t>
+  </si>
+  <si>
+    <t>ingresos</t>
+  </si>
+  <si>
+    <t>proyecto pequenio</t>
+  </si>
+  <si>
+    <t>proyecto mediano</t>
+  </si>
+  <si>
+    <t>proyecto grande</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5k </t>
+  </si>
+  <si>
+    <t>30k</t>
+  </si>
+  <si>
+    <t>75k</t>
   </si>
 </sst>
 </file>
@@ -92,12 +122,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{004A867A-0382-40B3-98A8-B18A58385743}">
-  <dimension ref="B3:C9"/>
+  <dimension ref="B3:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,41 +474,94 @@
     <col min="2" max="2" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="C4">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="C7" s="3">
+        <v>44105</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
+      <c r="C9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="2"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>